<commit_message>
Updated the excel structures
</commit_message>
<xml_diff>
--- a/backend/excels/Pelaajatilastot_tyhja.xlsx
+++ b/backend/excels/Pelaajatilastot_tyhja.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Player Totals" sheetId="1" state="visible" r:id="rId3"/>
@@ -173,7 +173,7 @@
     <t xml:space="preserve">Joukkue</t>
   </si>
   <si>
-    <t xml:space="preserve">PEL</t>
+    <t xml:space="preserve">Oma</t>
   </si>
   <si>
     <t xml:space="preserve">Vs.</t>
@@ -1250,8 +1250,8 @@
   </sheetPr>
   <dimension ref="A1:AR141"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T12" activeCellId="0" sqref="T12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N56" activeCellId="1" sqref="B34 N56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2722,7 +2722,7 @@
       <c r="D37" s="88" t="s">
         <v>52</v>
       </c>
-      <c r="E37" s="89" t="s">
+      <c r="E37" s="86" t="s">
         <v>50</v>
       </c>
       <c r="F37" s="87" t="s">
@@ -2740,7 +2740,7 @@
       <c r="J37" s="88" t="s">
         <v>52</v>
       </c>
-      <c r="K37" s="89" t="s">
+      <c r="K37" s="86" t="s">
         <v>50</v>
       </c>
       <c r="L37" s="87" t="s">
@@ -3025,7 +3025,7 @@
       <c r="D45" s="88" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="89" t="s">
+      <c r="E45" s="86" t="s">
         <v>50</v>
       </c>
       <c r="F45" s="87" t="s">
@@ -3043,7 +3043,7 @@
       <c r="J45" s="88" t="s">
         <v>52</v>
       </c>
-      <c r="K45" s="89" t="s">
+      <c r="K45" s="86" t="s">
         <v>50</v>
       </c>
       <c r="L45" s="87" t="s">
@@ -11052,8 +11052,8 @@
   </sheetPr>
   <dimension ref="A1:AR1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12052,7 +12052,7 @@
       <c r="A28" s="113" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="86" t="s">
         <v>50</v>
       </c>
       <c r="C28" s="114" t="s">
@@ -12061,7 +12061,7 @@
       <c r="D28" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E28" s="18" t="s">
+      <c r="E28" s="86" t="s">
         <v>50</v>
       </c>
       <c r="F28" s="22" t="s">
@@ -12070,7 +12070,7 @@
       <c r="G28" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H28" s="16" t="s">
+      <c r="H28" s="86" t="s">
         <v>50</v>
       </c>
       <c r="I28" s="114" t="s">
@@ -12079,7 +12079,7 @@
       <c r="J28" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="K28" s="18" t="s">
+      <c r="K28" s="86" t="s">
         <v>50</v>
       </c>
       <c r="L28" s="22" t="s">
@@ -12088,7 +12088,7 @@
       <c r="M28" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="N28" s="16" t="s">
+      <c r="N28" s="86" t="s">
         <v>50</v>
       </c>
       <c r="O28" s="114" t="s">
@@ -12266,7 +12266,7 @@
       <c r="A34" s="113" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="86" t="s">
         <v>50</v>
       </c>
       <c r="C34" s="114" t="s">
@@ -12275,7 +12275,7 @@
       <c r="D34" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E34" s="18" t="s">
+      <c r="E34" s="86" t="s">
         <v>50</v>
       </c>
       <c r="F34" s="22" t="s">
@@ -12284,7 +12284,7 @@
       <c r="G34" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H34" s="16" t="s">
+      <c r="H34" s="86" t="s">
         <v>50</v>
       </c>
       <c r="I34" s="114" t="s">
@@ -12293,7 +12293,7 @@
       <c r="J34" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="K34" s="18" t="s">
+      <c r="K34" s="86" t="s">
         <v>50</v>
       </c>
       <c r="L34" s="22" t="s">
@@ -12302,7 +12302,7 @@
       <c r="M34" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="N34" s="16" t="s">
+      <c r="N34" s="86" t="s">
         <v>50</v>
       </c>
       <c r="O34" s="114" t="s">

</xml_diff>

<commit_message>
Added team dashboard, keep alive improvements and readme (#42)
* Implemented the team dashboard page

* Cleaned up leftover todos and prints

* Final cleanup for portfolio

* Added readme

* improved backend coldstart avoidance

* 1. made dashboard cache team aware, 2.implemented eager loading to excel

* Updated the excel structures
</commit_message>
<xml_diff>
--- a/backend/excels/Pelaajatilastot_tyhja.xlsx
+++ b/backend/excels/Pelaajatilastot_tyhja.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Player Totals" sheetId="1" state="visible" r:id="rId3"/>
@@ -173,7 +173,7 @@
     <t xml:space="preserve">Joukkue</t>
   </si>
   <si>
-    <t xml:space="preserve">PEL</t>
+    <t xml:space="preserve">Oma</t>
   </si>
   <si>
     <t xml:space="preserve">Vs.</t>
@@ -1250,8 +1250,8 @@
   </sheetPr>
   <dimension ref="A1:AR141"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T12" activeCellId="0" sqref="T12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N56" activeCellId="1" sqref="B34 N56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2722,7 +2722,7 @@
       <c r="D37" s="88" t="s">
         <v>52</v>
       </c>
-      <c r="E37" s="89" t="s">
+      <c r="E37" s="86" t="s">
         <v>50</v>
       </c>
       <c r="F37" s="87" t="s">
@@ -2740,7 +2740,7 @@
       <c r="J37" s="88" t="s">
         <v>52</v>
       </c>
-      <c r="K37" s="89" t="s">
+      <c r="K37" s="86" t="s">
         <v>50</v>
       </c>
       <c r="L37" s="87" t="s">
@@ -3025,7 +3025,7 @@
       <c r="D45" s="88" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="89" t="s">
+      <c r="E45" s="86" t="s">
         <v>50</v>
       </c>
       <c r="F45" s="87" t="s">
@@ -3043,7 +3043,7 @@
       <c r="J45" s="88" t="s">
         <v>52</v>
       </c>
-      <c r="K45" s="89" t="s">
+      <c r="K45" s="86" t="s">
         <v>50</v>
       </c>
       <c r="L45" s="87" t="s">
@@ -11052,8 +11052,8 @@
   </sheetPr>
   <dimension ref="A1:AR1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12052,7 +12052,7 @@
       <c r="A28" s="113" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="86" t="s">
         <v>50</v>
       </c>
       <c r="C28" s="114" t="s">
@@ -12061,7 +12061,7 @@
       <c r="D28" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E28" s="18" t="s">
+      <c r="E28" s="86" t="s">
         <v>50</v>
       </c>
       <c r="F28" s="22" t="s">
@@ -12070,7 +12070,7 @@
       <c r="G28" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H28" s="16" t="s">
+      <c r="H28" s="86" t="s">
         <v>50</v>
       </c>
       <c r="I28" s="114" t="s">
@@ -12079,7 +12079,7 @@
       <c r="J28" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="K28" s="18" t="s">
+      <c r="K28" s="86" t="s">
         <v>50</v>
       </c>
       <c r="L28" s="22" t="s">
@@ -12088,7 +12088,7 @@
       <c r="M28" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="N28" s="16" t="s">
+      <c r="N28" s="86" t="s">
         <v>50</v>
       </c>
       <c r="O28" s="114" t="s">
@@ -12266,7 +12266,7 @@
       <c r="A34" s="113" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="86" t="s">
         <v>50</v>
       </c>
       <c r="C34" s="114" t="s">
@@ -12275,7 +12275,7 @@
       <c r="D34" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E34" s="18" t="s">
+      <c r="E34" s="86" t="s">
         <v>50</v>
       </c>
       <c r="F34" s="22" t="s">
@@ -12284,7 +12284,7 @@
       <c r="G34" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H34" s="16" t="s">
+      <c r="H34" s="86" t="s">
         <v>50</v>
       </c>
       <c r="I34" s="114" t="s">
@@ -12293,7 +12293,7 @@
       <c r="J34" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="K34" s="18" t="s">
+      <c r="K34" s="86" t="s">
         <v>50</v>
       </c>
       <c r="L34" s="22" t="s">
@@ -12302,7 +12302,7 @@
       <c r="M34" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="N34" s="16" t="s">
+      <c r="N34" s="86" t="s">
         <v>50</v>
       </c>
       <c r="O34" s="114" t="s">

</xml_diff>